<commit_message>
jocul X si O
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0F3FD2-8E6F-4E4A-A24A-381D4AABCB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464A4EE6-540D-4C57-ABA4-E38F873DDB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Proiect</t>
   </si>
@@ -79,6 +79,75 @@
   </si>
   <si>
     <t>săpt. 14</t>
+  </si>
+  <si>
+    <t>Madalin Blaj</t>
+  </si>
+  <si>
+    <t>Luca Bulea</t>
+  </si>
+  <si>
+    <t>Bianca Nicorici</t>
+  </si>
+  <si>
+    <t>Noelia Sfrangeu</t>
+  </si>
+  <si>
+    <t>Razvan Ardeli</t>
+  </si>
+  <si>
+    <t>Nuria Girz</t>
+  </si>
+  <si>
+    <t>Adina Pop</t>
+  </si>
+  <si>
+    <t>David Florea</t>
+  </si>
+  <si>
+    <t>Erik Lazin</t>
+  </si>
+  <si>
+    <t>Cristina Nemcea</t>
+  </si>
+  <si>
+    <t>Renata Halasz</t>
+  </si>
+  <si>
+    <t>Georgiana Galea</t>
+  </si>
+  <si>
+    <t>Daria Petre</t>
+  </si>
+  <si>
+    <t>Roberto Lazar</t>
+  </si>
+  <si>
+    <t>Catalin Lazar</t>
+  </si>
+  <si>
+    <t>Nicolae Goie</t>
+  </si>
+  <si>
+    <t>David Klein</t>
+  </si>
+  <si>
+    <t>Roland Roman</t>
+  </si>
+  <si>
+    <t>Vlad Varkonyi</t>
+  </si>
+  <si>
+    <t>Andrei Negrut</t>
+  </si>
+  <si>
+    <t>Andreea Farcas</t>
+  </si>
+  <si>
+    <t>Bianca Abrudan</t>
+  </si>
+  <si>
+    <t>Vanesa Crepce</t>
   </si>
 </sst>
 </file>
@@ -614,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -682,8 +751,12 @@
       </c>
     </row>
     <row r="3" spans="2:19">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -698,250 +771,338 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f t="shared" ref="Q3:Q50" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>0</v>
+        <f t="shared" ref="Q3:Q11" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>1</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="9"/>
     </row>
     <row r="4" spans="2:19">
-      <c r="B4" s="3"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19">
-      <c r="B5" s="3"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="3"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="12"/>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="3"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
     </row>
     <row r="8" spans="2:19">
-      <c r="B8" s="3"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:19">
-      <c r="B9" s="3"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="3"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="Q12:Q50" si="1">C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>1</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="3"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="3"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="3"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="3"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="3"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
-      <c r="B18" s="3"/>
-      <c r="C18" s="10"/>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="2:19">
-      <c r="B19" s="3"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19">
-      <c r="B20" s="3"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="3"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="3"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="3"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="3"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="3"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
@@ -951,7 +1112,7 @@
       <c r="C26" s="10"/>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R26" s="12"/>
@@ -962,7 +1123,7 @@
       <c r="C27" s="10"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R27" s="12"/>
@@ -973,7 +1134,7 @@
       <c r="C28" s="10"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="12"/>
@@ -984,7 +1145,7 @@
       <c r="C29" s="10"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="12"/>
@@ -995,7 +1156,7 @@
       <c r="C30" s="10"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="12"/>
@@ -1006,7 +1167,7 @@
       <c r="C31" s="10"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R31" s="12"/>
@@ -1017,7 +1178,7 @@
       <c r="C32" s="10"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R32" s="12"/>
@@ -1028,7 +1189,7 @@
       <c r="C33" s="10"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R33" s="12"/>
@@ -1039,7 +1200,7 @@
       <c r="C34" s="10"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R34" s="12"/>
@@ -1050,7 +1211,7 @@
       <c r="C35" s="10"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R35" s="12"/>
@@ -1061,7 +1222,7 @@
       <c r="C36" s="10"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R36" s="12"/>
@@ -1072,7 +1233,7 @@
       <c r="C37" s="10"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R37" s="12"/>
@@ -1083,7 +1244,7 @@
       <c r="C38" s="10"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1094,7 +1255,7 @@
       <c r="C39" s="10"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1105,7 +1266,7 @@
       <c r="C40" s="10"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1116,7 +1277,7 @@
       <c r="C41" s="10"/>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1127,7 +1288,7 @@
       <c r="C42" s="10"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1138,7 +1299,7 @@
       <c r="C43" s="10"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1149,7 +1310,7 @@
       <c r="C44" s="10"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1160,7 +1321,7 @@
       <c r="C45" s="10"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1171,7 +1332,7 @@
       <c r="C46" s="10"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1182,7 +1343,7 @@
       <c r="C47" s="10"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1193,7 +1354,7 @@
       <c r="C48" s="10"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1204,7 +1365,7 @@
       <c r="C49" s="10"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="14"/>
@@ -1227,13 +1388,16 @@
       <c r="O50" s="19"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="21"/>
       <c r="S50" s="22"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S11">
+    <sortCondition ref="B3:B11"/>
+  </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>4</formula>

</xml_diff>

<commit_message>
Am adaugat functionalitate pentru salvare si citire din fisier pentru numarul de castiguri ale lui X si ale lui O
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464A4EE6-540D-4C57-ABA4-E38F873DDB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EDC0A-C959-4E25-A947-E5ADA3772B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -684,7 +684,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Laborator 12.02.2024 - Matrici
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54EDC0A-C959-4E25-A947-E5ADA3772B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781DB558-9119-41AA-8815-44CA656A1A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Proiect</t>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>Vanesa Crepce</t>
+  </si>
+  <si>
+    <t>Aniko Vieriu</t>
+  </si>
+  <si>
+    <t>Diana Lazea</t>
+  </si>
+  <si>
+    <t>Cosmin Chira</t>
+  </si>
+  <si>
+    <t>Vlad Chis</t>
+  </si>
+  <si>
+    <t>Patrick Tocut</t>
+  </si>
+  <si>
+    <t>Alexandru Lupse</t>
   </si>
 </sst>
 </file>
@@ -683,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -757,7 +775,9 @@
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -771,22 +791,23 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f t="shared" ref="Q3:Q11" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>1</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>2</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="9"/>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="10" t="b">
+        <v>46</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>1</v>
       </c>
       <c r="R4" s="12"/>
@@ -794,29 +815,32 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R5" s="12"/>
-      <c r="S5" s="13"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>2</v>
+      </c>
+      <c r="R5" s="14"/>
+      <c r="S5" s="15"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C6" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
       <c r="R6" s="12"/>
@@ -824,14 +848,15 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="10" t="b">
+        <v>41</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
-        <f t="shared" si="0"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
         <v>1</v>
       </c>
       <c r="R7" s="12"/>
@@ -839,29 +864,32 @@
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>2</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>1</v>
       </c>
       <c r="R9" s="12"/>
@@ -869,29 +897,33 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>2</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10" t="b">
+        <v>43</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>1</v>
       </c>
       <c r="R11" s="12"/>
@@ -906,7 +938,7 @@
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
-        <f t="shared" ref="Q12:Q50" si="1">C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>1</v>
       </c>
       <c r="R12" s="12"/>
@@ -914,89 +946,102 @@
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>2</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>2</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C15" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>2</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="10" t="b">
+        <v>42</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R16" s="14"/>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="12"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C17" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>2</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C18" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
-        <f t="shared" si="1"/>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
         <v>1</v>
       </c>
       <c r="R18" s="12"/>
@@ -1004,14 +1049,14 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C19" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
-        <f t="shared" si="1"/>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
         <v>1</v>
       </c>
       <c r="R19" s="12"/>
@@ -1019,14 +1064,14 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
-        <f t="shared" si="1"/>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
         <v>1</v>
       </c>
       <c r="R20" s="12"/>
@@ -1034,14 +1079,14 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C21" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
-        <f t="shared" si="1"/>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
         <v>1</v>
       </c>
       <c r="R21" s="12"/>
@@ -1049,44 +1094,51 @@
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>2</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C23" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R23" s="14"/>
-      <c r="S23" s="15"/>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>2</v>
+      </c>
+      <c r="R23" s="12"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="10" t="b">
+        <v>45</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
-        <f t="shared" si="1"/>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
         <v>1</v>
       </c>
       <c r="R24" s="12"/>
@@ -1094,81 +1146,115 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C25" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>2</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="3"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>2</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19">
-      <c r="B27" s="3"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="12"/>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>1</v>
+      </c>
+      <c r="R27" s="14"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="3"/>
-      <c r="C28" s="10"/>
+      <c r="B28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>2</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="3"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>1</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C30" s="10"/>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="B31" s="3"/>
-      <c r="C31" s="10"/>
+      <c r="B31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>1</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
@@ -1178,7 +1264,7 @@
       <c r="C32" s="10"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q12:Q50" si="0">C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
         <v>0</v>
       </c>
       <c r="R32" s="12"/>
@@ -1189,7 +1275,7 @@
       <c r="C33" s="10"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R33" s="12"/>
@@ -1200,7 +1286,7 @@
       <c r="C34" s="10"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R34" s="12"/>
@@ -1211,7 +1297,7 @@
       <c r="C35" s="10"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R35" s="12"/>
@@ -1222,7 +1308,7 @@
       <c r="C36" s="10"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R36" s="12"/>
@@ -1233,7 +1319,7 @@
       <c r="C37" s="10"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R37" s="12"/>
@@ -1244,7 +1330,7 @@
       <c r="C38" s="10"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1255,7 +1341,7 @@
       <c r="C39" s="10"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1266,7 +1352,7 @@
       <c r="C40" s="10"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1277,7 +1363,7 @@
       <c r="C41" s="10"/>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1288,7 +1374,7 @@
       <c r="C42" s="10"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1299,7 +1385,7 @@
       <c r="C43" s="10"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1310,7 +1396,7 @@
       <c r="C44" s="10"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1321,7 +1407,7 @@
       <c r="C45" s="10"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1332,7 +1418,7 @@
       <c r="C46" s="10"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1343,7 +1429,7 @@
       <c r="C47" s="10"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1354,7 +1440,7 @@
       <c r="C48" s="10"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1365,7 +1451,7 @@
       <c r="C49" s="10"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R49" s="14"/>
@@ -1388,15 +1474,15 @@
       <c r="O50" s="19"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R50" s="21"/>
       <c r="S50" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S11">
-    <sortCondition ref="B3:B11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S31">
+    <sortCondition ref="B31"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 14.03.2024 - Fake Photoshop. Gray scale, Complementary, Contrast, Blur.
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781DB558-9119-41AA-8815-44CA656A1A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300D242F-CF2D-43A7-BFEB-FC2FC900DFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Proiect</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Alexandru Lupse</t>
+  </si>
+  <si>
+    <t>Raluca Veres</t>
+  </si>
+  <si>
+    <t>Gabriela Maghear</t>
+  </si>
+  <si>
+    <t>Sebastian Pop</t>
   </si>
 </sst>
 </file>
@@ -701,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -791,7 +800,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q31" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="8"/>
@@ -805,10 +814,13 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="13"/>
@@ -825,7 +837,7 @@
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R5" s="14"/>
@@ -840,7 +852,7 @@
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R6" s="12"/>
@@ -854,10 +866,13 @@
       <c r="D7" t="b">
         <v>1</v>
       </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
@@ -872,10 +887,13 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
@@ -889,7 +907,7 @@
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R9" s="12"/>
@@ -907,7 +925,7 @@
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R10" s="12"/>
@@ -923,7 +941,7 @@
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R11" s="12"/>
@@ -938,7 +956,7 @@
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R12" s="12"/>
@@ -954,10 +972,13 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
@@ -974,7 +995,7 @@
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R14" s="12"/>
@@ -992,7 +1013,7 @@
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R15" s="12"/>
@@ -1008,7 +1029,7 @@
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R16" s="12"/>
@@ -1026,7 +1047,7 @@
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R17" s="12"/>
@@ -1039,10 +1060,13 @@
       <c r="C18" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
@@ -1054,10 +1078,13 @@
       <c r="C19" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
@@ -1069,10 +1096,13 @@
       <c r="C20" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
@@ -1086,7 +1116,7 @@
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R21" s="12"/>
@@ -1102,10 +1132,13 @@
       <c r="D22" t="b">
         <v>1</v>
       </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
@@ -1122,7 +1155,7 @@
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R23" s="12"/>
@@ -1138,7 +1171,7 @@
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R24" s="12"/>
@@ -1154,10 +1187,13 @@
       <c r="D25" t="b">
         <v>1</v>
       </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
@@ -1172,10 +1208,13 @@
       <c r="D26" t="b">
         <v>1</v>
       </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
@@ -1189,7 +1228,7 @@
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R27" s="14"/>
@@ -1207,7 +1246,7 @@
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R28" s="12"/>
@@ -1220,10 +1259,13 @@
       <c r="C29" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
@@ -1238,7 +1280,7 @@
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R30" s="12"/>
@@ -1253,41 +1295,56 @@
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19">
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C32" s="10"/>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
-        <f t="shared" ref="Q12:Q50" si="0">C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>0</v>
+        <f t="shared" ref="Q32:Q50" si="1">C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>1</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
     </row>
     <row r="33" spans="2:19">
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="C33" s="10"/>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
     </row>
     <row r="34" spans="2:19">
-      <c r="B34" s="3"/>
+      <c r="B34" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C34" s="10"/>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
@@ -1297,7 +1354,7 @@
       <c r="C35" s="10"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R35" s="12"/>
@@ -1308,7 +1365,7 @@
       <c r="C36" s="10"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R36" s="12"/>
@@ -1319,7 +1376,7 @@
       <c r="C37" s="10"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R37" s="12"/>
@@ -1330,7 +1387,7 @@
       <c r="C38" s="10"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1341,7 +1398,7 @@
       <c r="C39" s="10"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1352,7 +1409,7 @@
       <c r="C40" s="10"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1363,7 +1420,7 @@
       <c r="C41" s="10"/>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1374,7 +1431,7 @@
       <c r="C42" s="10"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1385,7 +1442,7 @@
       <c r="C43" s="10"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1396,7 +1453,7 @@
       <c r="C44" s="10"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1407,7 +1464,7 @@
       <c r="C45" s="10"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1418,7 +1475,7 @@
       <c r="C46" s="10"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1429,7 +1486,7 @@
       <c r="C47" s="10"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1440,7 +1497,7 @@
       <c r="C48" s="10"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1451,7 +1508,7 @@
       <c r="C49" s="10"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="14"/>
@@ -1474,7 +1531,7 @@
       <c r="O50" s="19"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="21"/>

</xml_diff>

<commit_message>
Laborator 19.03.2024 - am inceput jocul 2048. Am generat tile-urile vizual si le-am facut sa mearga spre dreapta.
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300D242F-CF2D-43A7-BFEB-FC2FC900DFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42886D4-9B98-4F09-B86C-742566F91273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Proiect</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Sebastian Pop</t>
+  </si>
+  <si>
+    <t>Luminita Hava</t>
+  </si>
+  <si>
+    <t>Victor Balaj</t>
+  </si>
+  <si>
+    <t>Emanuel Socaciu</t>
   </si>
 </sst>
 </file>
@@ -710,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +797,9 @@
         <v>1</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -800,8 +811,8 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f t="shared" ref="Q3:Q31" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>2</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>3</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="9"/>
@@ -817,10 +828,13 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <v>3</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="13"/>
@@ -835,10 +849,13 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>3</v>
       </c>
       <c r="R5" s="14"/>
       <c r="S5" s="15"/>
@@ -852,7 +869,7 @@
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
       <c r="R6" s="12"/>
@@ -869,10 +886,13 @@
       <c r="E7" t="b">
         <v>1</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>3</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
@@ -890,10 +910,13 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>4</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
@@ -907,7 +930,7 @@
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>1</v>
       </c>
       <c r="R9" s="12"/>
@@ -925,7 +948,7 @@
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
-        <f t="shared" si="0"/>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
         <v>2</v>
       </c>
       <c r="R10" s="12"/>
@@ -941,7 +964,7 @@
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>1</v>
       </c>
       <c r="R11" s="12"/>
@@ -954,10 +977,13 @@
       <c r="C12" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>2</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13"/>
@@ -975,10 +1001,13 @@
       <c r="E13" t="b">
         <v>1</v>
       </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>4</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
@@ -993,10 +1022,13 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>3</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
@@ -1011,10 +1043,13 @@
       <c r="D15" t="b">
         <v>1</v>
       </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>3</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
@@ -1029,7 +1064,7 @@
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
-        <f t="shared" si="0"/>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
         <v>1</v>
       </c>
       <c r="R16" s="12"/>
@@ -1037,53 +1072,55 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>1</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="E18" t="b">
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>3</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C19" s="10"/>
       <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
-        <f t="shared" si="0"/>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
         <v>2</v>
       </c>
       <c r="R19" s="12"/>
@@ -1091,7 +1128,7 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C20" s="10" t="b">
         <v>1</v>
@@ -1101,7 +1138,7 @@
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
-        <f t="shared" si="0"/>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
         <v>2</v>
       </c>
       <c r="R20" s="12"/>
@@ -1109,53 +1146,51 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C21" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>2</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
+        <v>50</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>1</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C23" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D23" t="b">
+      <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
-        <f t="shared" si="0"/>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
         <v>2</v>
       </c>
       <c r="R23" s="12"/>
@@ -1163,15 +1198,14 @@
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" t="b">
+        <v>33</v>
+      </c>
+      <c r="C24" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
-        <f t="shared" si="0"/>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
         <v>1</v>
       </c>
       <c r="R24" s="12"/>
@@ -1179,7 +1213,7 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="10" t="b">
         <v>1</v>
@@ -1192,7 +1226,7 @@
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
-        <f t="shared" si="0"/>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
         <v>3</v>
       </c>
       <c r="R25" s="12"/>
@@ -1200,7 +1234,7 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C26" s="10" t="b">
         <v>1</v>
@@ -1208,12 +1242,12 @@
       <c r="D26" t="b">
         <v>1</v>
       </c>
-      <c r="E26" t="b">
+      <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
-        <f t="shared" si="0"/>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
         <v>3</v>
       </c>
       <c r="R26" s="12"/>
@@ -1221,32 +1255,37 @@
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="10" t="b">
+        <v>45</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R27" s="14"/>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>2</v>
+      </c>
+      <c r="R27" s="12"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
+        <v>47</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
-        <f t="shared" si="0"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
         <v>2</v>
       </c>
       <c r="R28" s="12"/>
@@ -1254,72 +1293,91 @@
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C29" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
       <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>4</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>4</v>
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C31" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R31" s="12"/>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>1</v>
+      </c>
+      <c r="R31" s="14"/>
       <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="E32" t="b">
+        <v>35</v>
+      </c>
+      <c r="C32" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
-        <f t="shared" ref="Q32:Q50" si="1">C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>1</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>3</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" s="10"/>
       <c r="E33" t="b">
@@ -1327,7 +1385,7 @@
       </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
-        <f t="shared" si="1"/>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
         <v>1</v>
       </c>
       <c r="R33" s="12"/>
@@ -1335,49 +1393,71 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="C34" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>3</v>
       </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
     </row>
     <row r="35" spans="2:19">
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C35" s="10"/>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>1</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="2:19">
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C36" s="10"/>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>2</v>
       </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
     </row>
     <row r="37" spans="2:19">
-      <c r="B37" s="3"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>1</v>
       </c>
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
@@ -1387,7 +1467,7 @@
       <c r="C38" s="10"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q32:Q50" si="0">C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
         <v>0</v>
       </c>
       <c r="R38" s="12"/>
@@ -1398,7 +1478,7 @@
       <c r="C39" s="10"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R39" s="12"/>
@@ -1409,7 +1489,7 @@
       <c r="C40" s="10"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R40" s="12"/>
@@ -1420,7 +1500,7 @@
       <c r="C41" s="10"/>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R41" s="12"/>
@@ -1431,7 +1511,7 @@
       <c r="C42" s="10"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1442,7 +1522,7 @@
       <c r="C43" s="10"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="12"/>
@@ -1453,7 +1533,7 @@
       <c r="C44" s="10"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="12"/>
@@ -1464,7 +1544,7 @@
       <c r="C45" s="10"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1475,7 +1555,7 @@
       <c r="C46" s="10"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R46" s="12"/>
@@ -1486,7 +1566,7 @@
       <c r="C47" s="10"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R47" s="12"/>
@@ -1497,7 +1577,7 @@
       <c r="C48" s="10"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1508,7 +1588,7 @@
       <c r="C49" s="10"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R49" s="14"/>
@@ -1531,15 +1611,15 @@
       <c r="O50" s="19"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R50" s="21"/>
       <c r="S50" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S31">
-    <sortCondition ref="B31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S37">
+    <sortCondition ref="B37"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 21.03.2024 - Greedy, probleme rezolvate eficient
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42886D4-9B98-4F09-B86C-742566F91273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8203F5D-6971-452C-A817-EB356671BF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Proiect</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Emanuel Socaciu</t>
+  </si>
+  <si>
+    <t>Andrei Tig</t>
+  </si>
+  <si>
+    <t>Victor Pitirici</t>
+  </si>
+  <si>
+    <t>Alexandra Iovan</t>
+  </si>
+  <si>
+    <t>David Nadis</t>
   </si>
 </sst>
 </file>
@@ -720,7 +732,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,34 +831,29 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
         <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="b">
@@ -857,33 +864,35 @@
         <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
         <v>3</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
         <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>1</v>
-      </c>
-      <c r="R6" s="12"/>
-      <c r="S6" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="R6" s="14"/>
+      <c r="S6" s="15"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
+        <v>37</v>
+      </c>
+      <c r="C7" s="10" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="b">
@@ -892,92 +901,99 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C8" s="10"/>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10" t="b">
+        <v>41</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C10" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" t="b">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C12" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F12" t="b">
+      <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="11"/>
@@ -990,36 +1006,25 @@
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C13" s="10"/>
       <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="b">
@@ -1028,19 +1033,22 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="F15" t="b">
@@ -1049,234 +1057,242 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="C16" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="C17" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C18" s="10"/>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
+      <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
+        <v>52</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C21" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="E21" t="b">
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="10"/>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C23" s="10" t="b">
         <v>1</v>
       </c>
       <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R23" s="12"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C24" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
         <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
+        <v>50</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C26" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" t="b">
+      <c r="E26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" t="b">
+        <v>33</v>
+      </c>
+      <c r="C27" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
       <c r="E28" t="b">
         <v>1</v>
       </c>
@@ -1286,22 +1302,19 @@
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C29" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
         <v>1</v>
       </c>
       <c r="F29" t="b">
@@ -1310,22 +1323,17 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
         <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C30" s="10"/>
       <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" t="b">
         <v>1</v>
       </c>
       <c r="F30" t="b">
@@ -1334,34 +1342,41 @@
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="10" t="b">
+        <v>47</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
         <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>1</v>
-      </c>
-      <c r="R31" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="R31" s="12"/>
       <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C32" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
         <v>1</v>
       </c>
       <c r="F32" t="b">
@@ -1370,70 +1385,77 @@
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
         <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="C33" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
       <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
         <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C34" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
         <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>3</v>
-      </c>
-      <c r="R34" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="R34" s="14"/>
       <c r="S34" s="13"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="C35" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
       <c r="F35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C36" s="10"/>
-      <c r="D36" t="b">
+      <c r="E36" t="b">
         <v>1</v>
       </c>
       <c r="F36" t="b">
@@ -1449,59 +1471,90 @@
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C37" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
         <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
     </row>
     <row r="38" spans="2:19">
-      <c r="B38" s="3"/>
+      <c r="B38" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C38" s="10"/>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
-        <f t="shared" ref="Q32:Q50" si="0">C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>0</v>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>1</v>
       </c>
       <c r="R38" s="12"/>
       <c r="S38" s="13"/>
     </row>
     <row r="39" spans="2:19">
-      <c r="B39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="C39" s="10"/>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>1</v>
       </c>
       <c r="R39" s="12"/>
       <c r="S39" s="13"/>
     </row>
     <row r="40" spans="2:19">
-      <c r="B40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C40" s="10"/>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <v>2</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="3"/>
-      <c r="C41" s="10"/>
+      <c r="B41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>2</v>
       </c>
       <c r="R41" s="12"/>
       <c r="S41" s="13"/>
@@ -1511,7 +1564,7 @@
       <c r="C42" s="10"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q38:Q50" si="0">C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
         <v>0</v>
       </c>
       <c r="R42" s="12"/>
@@ -1618,8 +1671,8 @@
       <c r="S50" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S37">
-    <sortCondition ref="B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S41">
+    <sortCondition ref="B41"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 26.03.2024 - toate miscarile tile-urilor facute si afisatul numerelor
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8203F5D-6971-452C-A817-EB356671BF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E832BB30-E204-4526-9E1B-3AAB663FE7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Proiect</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>David Nadis</t>
+  </si>
+  <si>
+    <t>Beniamin Vutan</t>
+  </si>
+  <si>
+    <t>Danut Jurjut</t>
+  </si>
+  <si>
+    <t>Karoli Forrai</t>
   </si>
 </sst>
 </file>
@@ -732,7 +741,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,7 +821,9 @@
       <c r="F3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -824,7 +835,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
         <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="9"/>
@@ -859,10 +870,13 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
         <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
@@ -880,10 +894,13 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
         <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" s="14"/>
       <c r="S6" s="15"/>
@@ -898,10 +915,13 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
@@ -946,88 +966,98 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
+        <v>57</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C11" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
       <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C12" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D12" t="b">
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="C13" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
+        <v>43</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="11"/>
@@ -1040,15 +1070,9 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="F15" t="b">
@@ -1057,40 +1081,38 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
+        <v>58</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="F17" t="b">
@@ -1099,46 +1121,59 @@
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="C18" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
       <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="C19" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C20" s="10"/>
       <c r="F20" t="b">
@@ -1154,76 +1189,75 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C21" s="10"/>
       <c r="D21" t="b">
         <v>1</v>
       </c>
-      <c r="F21" t="b">
+      <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C23" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="E23" t="b">
+      <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R23" s="12"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C24" s="10"/>
       <c r="E24" t="b">
         <v>1</v>
       </c>
       <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="11"/>
@@ -1236,88 +1270,92 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="C25" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="b">
+        <v>59</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="G26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C27" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C28" s="10"/>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C29" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="b">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="11"/>
@@ -1330,45 +1368,49 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="b">
+        <v>33</v>
+      </c>
+      <c r="C30" s="10" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C31" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
       <c r="E31" t="b">
         <v>1</v>
       </c>
       <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
         <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" s="10" t="b">
         <v>1</v>
@@ -1376,10 +1418,10 @@
       <c r="D32" t="b">
         <v>1</v>
       </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
       <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="11"/>
@@ -1392,15 +1434,10 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C33" s="10"/>
       <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" t="b">
         <v>1</v>
       </c>
       <c r="F33" t="b">
@@ -1409,29 +1446,36 @@
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
         <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="10" t="b">
+        <v>47</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
         <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>1</v>
-      </c>
-      <c r="R34" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="R34" s="12"/>
       <c r="S34" s="13"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C35" s="10" t="b">
         <v>1</v>
@@ -1439,22 +1483,33 @@
       <c r="D35" t="b">
         <v>1</v>
       </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
       <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="C36" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
       <c r="E36" t="b">
         <v>1</v>
       </c>
@@ -1464,130 +1519,167 @@
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
         <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C37" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
+      <c r="G37" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
         <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>3</v>
-      </c>
-      <c r="R37" s="12"/>
+        <v>2</v>
+      </c>
+      <c r="R37" s="14"/>
       <c r="S37" s="13"/>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="C38" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
       <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
         <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R38" s="12"/>
       <c r="S38" s="13"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C39" s="10"/>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
       <c r="F39" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
         <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R39" s="12"/>
       <c r="S39" s="13"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" t="b">
+        <v>40</v>
+      </c>
+      <c r="C40" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
         <v>1</v>
       </c>
       <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
         <v>1</v>
       </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
         <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C41" s="10"/>
       <c r="F41" t="b">
         <v>1</v>
       </c>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
         <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R41" s="12"/>
       <c r="S41" s="13"/>
     </row>
     <row r="42" spans="2:19">
-      <c r="B42" s="3"/>
+      <c r="B42" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="C42" s="10"/>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f t="shared" ref="Q38:Q50" si="0">C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>0</v>
+        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <v>1</v>
       </c>
       <c r="R42" s="12"/>
       <c r="S42" s="13"/>
     </row>
     <row r="43" spans="2:19">
-      <c r="B43" s="3"/>
+      <c r="B43" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C43" s="10"/>
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <v>3</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="13"/>
     </row>
     <row r="44" spans="2:19">
-      <c r="B44" s="16"/>
-      <c r="C44" s="10"/>
+      <c r="B44" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
+        <v>3</v>
       </c>
       <c r="R44" s="12"/>
       <c r="S44" s="13"/>
@@ -1597,7 +1689,7 @@
       <c r="C45" s="10"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q42:Q50" si="0">C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
         <v>0</v>
       </c>
       <c r="R45" s="12"/>
@@ -1671,8 +1763,8 @@
       <c r="S50" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S41">
-    <sortCondition ref="B41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S44">
+    <sortCondition ref="B44"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 28.03.2024 - Problemele de la partial
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E832BB30-E204-4526-9E1B-3AAB663FE7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F0DDE9-0864-43C8-BD1A-917B69FD0FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Proiect</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Karoli Forrai</t>
+  </si>
+  <si>
+    <t>Gabriel Talmazan</t>
+  </si>
+  <si>
+    <t>Stefan Tulvan</t>
+  </si>
+  <si>
+    <t>Daniel Oistric</t>
   </si>
 </sst>
 </file>
@@ -740,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,10 +857,13 @@
       <c r="F4" t="b">
         <v>1</v>
       </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
         <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="13"/>
@@ -1088,7 +1100,7 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C16" s="10"/>
       <c r="G16" t="b">
@@ -1104,31 +1116,23 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
+        <v>58</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C18" s="10" t="b">
         <v>1</v>
@@ -1136,10 +1140,10 @@
       <c r="D18" t="b">
         <v>1</v>
       </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
       <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="11"/>
@@ -1152,7 +1156,7 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C19" s="10" t="b">
         <v>1</v>
@@ -1161,97 +1165,102 @@
         <v>1</v>
       </c>
       <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="C20" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
       <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" t="b">
+      <c r="F21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="F22" t="b">
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C23" s="10"/>
       <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R23" s="12"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="E24" t="b">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="F24" t="b">
@@ -1263,51 +1272,52 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
         <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="b">
+        <v>60</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="G25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C26" s="10"/>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
       <c r="G26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C27" s="10" t="b">
         <v>1</v>
@@ -1316,25 +1326,22 @@
         <v>1</v>
       </c>
       <c r="F27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="F28" t="b">
+      <c r="G28" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="11"/>
@@ -1347,12 +1354,15 @@
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="10" t="b">
         <v>1</v>
       </c>
       <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
         <v>1</v>
       </c>
       <c r="G29" t="b">
@@ -1361,16 +1371,17 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
         <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="10" t="b">
+        <v>50</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="F30" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="11"/>
@@ -1383,18 +1394,12 @@
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C31" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
       <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" t="b">
         <v>1</v>
       </c>
       <c r="G31" t="b">
@@ -1403,60 +1408,61 @@
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
         <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C32" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
         <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C33" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
       <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
         <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="E34" t="b">
+        <v>23</v>
+      </c>
+      <c r="C34" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="F34" t="b">
@@ -1468,67 +1474,66 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
         <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C35" s="10"/>
       <c r="D35" t="b">
         <v>1</v>
       </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
       <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C36" s="10"/>
       <c r="E36" t="b">
         <v>1</v>
       </c>
       <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
         <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C37" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
         <v>1</v>
       </c>
       <c r="G37" t="b">
@@ -1537,19 +1542,22 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
         <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>2</v>
-      </c>
-      <c r="R37" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="R37" s="12"/>
       <c r="S37" s="13"/>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C38" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
         <v>1</v>
       </c>
       <c r="F38" t="b">
@@ -1561,20 +1569,19 @@
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
         <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R38" s="12"/>
       <c r="S38" s="13"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
+        <v>31</v>
+      </c>
+      <c r="C39" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="11"/>
@@ -1582,17 +1589,17 @@
         <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
         <v>2</v>
       </c>
-      <c r="R39" s="12"/>
+      <c r="R39" s="14"/>
       <c r="S39" s="13"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C40" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="E40" t="b">
+      <c r="D40" t="b">
         <v>1</v>
       </c>
       <c r="F40" t="b">
@@ -1611,26 +1618,29 @@
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C41" s="10"/>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
       <c r="F41" t="b">
         <v>1</v>
       </c>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
         <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R41" s="12"/>
       <c r="S41" s="13"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C42" s="10"/>
-      <c r="F42" t="b">
+      <c r="G42" t="b">
         <v>1</v>
       </c>
       <c r="P42" s="11"/>
@@ -1643,10 +1653,12 @@
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" t="b">
+        <v>40</v>
+      </c>
+      <c r="C43" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" t="b">
         <v>1</v>
       </c>
       <c r="F43" t="b">
@@ -1658,61 +1670,85 @@
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
         <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="13"/>
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C44" s="10"/>
       <c r="F44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" t="b">
         <v>1</v>
       </c>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
         <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R44" s="12"/>
       <c r="S44" s="13"/>
     </row>
     <row r="45" spans="2:19">
-      <c r="B45" s="3"/>
+      <c r="B45" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="C45" s="10"/>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f t="shared" ref="Q42:Q50" si="0">C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
-        <v>0</v>
+        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <v>2</v>
       </c>
       <c r="R45" s="12"/>
       <c r="S45" s="13"/>
     </row>
     <row r="46" spans="2:19">
-      <c r="B46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C46" s="10"/>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <v>3</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13"/>
     </row>
     <row r="47" spans="2:19">
-      <c r="B47" s="17"/>
-      <c r="C47" s="10"/>
+      <c r="B47" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <v>3</v>
       </c>
       <c r="R47" s="12"/>
       <c r="S47" s="13"/>
@@ -1722,7 +1758,7 @@
       <c r="C48" s="10"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q45:Q50" si="0">C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1763,8 +1799,8 @@
       <c r="S50" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S44">
-    <sortCondition ref="B44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S47">
+    <sortCondition ref="B47"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 02.04.2024 - Am rezolvat un bug al jocului: nu mai putem face "miscari goale" - daca tasta pe care am apasat-o nu a schimbat nimic, nu generam un nou Tile. Am facut posibilitatea de a castiga, si am separat codul pe mai multe clase - cu o structura similara cu structura pe care o vom face la urmatorul joc
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F0DDE9-0864-43C8-BD1A-917B69FD0FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAEF8E2-20B4-44A6-8321-DEB565B1EF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -750,7 +750,7 @@
   <dimension ref="B2:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -843,7 +843,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q47" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>4</v>
       </c>
       <c r="R3" s="8"/>
@@ -860,10 +860,13 @@
       <c r="G4" t="b">
         <v>1</v>
       </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R4" s="12"/>
       <c r="S4" s="13"/>
@@ -885,10 +888,13 @@
       <c r="G5" t="b">
         <v>1</v>
       </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
@@ -911,7 +917,7 @@
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R6" s="14"/>
@@ -932,7 +938,7 @@
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R7" s="12"/>
@@ -948,7 +954,7 @@
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R8" s="12"/>
@@ -970,7 +976,7 @@
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R9" s="12"/>
@@ -986,7 +992,7 @@
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R10" s="12"/>
@@ -1011,10 +1017,13 @@
       <c r="G11" t="b">
         <v>1</v>
       </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13"/>
@@ -1034,7 +1043,7 @@
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R12" s="12"/>
@@ -1053,10 +1062,13 @@
       <c r="G13" t="b">
         <v>1</v>
       </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
@@ -1074,7 +1086,7 @@
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R14" s="12"/>
@@ -1092,7 +1104,7 @@
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R15" s="12"/>
@@ -1108,7 +1120,7 @@
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R16" s="12"/>
@@ -1124,7 +1136,7 @@
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R17" s="12"/>
@@ -1146,10 +1158,13 @@
       <c r="F18" t="b">
         <v>1</v>
       </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
@@ -1170,10 +1185,13 @@
       <c r="G19" t="b">
         <v>1</v>
       </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
@@ -1196,7 +1214,7 @@
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R20" s="12"/>
@@ -1212,7 +1230,7 @@
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R21" s="12"/>
@@ -1229,10 +1247,13 @@
       <c r="G22" t="b">
         <v>1</v>
       </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
@@ -1245,10 +1266,13 @@
       <c r="F23" t="b">
         <v>1</v>
       </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="7">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R23" s="12"/>
       <c r="S23" s="13"/>
@@ -1269,10 +1293,13 @@
       <c r="G24" t="b">
         <v>1</v>
       </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
@@ -1287,7 +1314,7 @@
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R25" s="12"/>
@@ -1307,10 +1334,13 @@
       <c r="G26" t="b">
         <v>1</v>
       </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
@@ -1328,10 +1358,13 @@
       <c r="F27" t="b">
         <v>1</v>
       </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="13"/>
@@ -1346,7 +1379,7 @@
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R28" s="12"/>
@@ -1368,10 +1401,13 @@
       <c r="G29" t="b">
         <v>1</v>
       </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
@@ -1386,7 +1422,7 @@
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R30" s="12"/>
@@ -1407,7 +1443,7 @@
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R31" s="12"/>
@@ -1422,7 +1458,7 @@
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R32" s="12"/>
@@ -1449,7 +1485,7 @@
       </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R33" s="12"/>
@@ -1473,7 +1509,7 @@
       </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R34" s="12"/>
@@ -1490,10 +1526,13 @@
       <c r="F35" t="b">
         <v>1</v>
       </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
@@ -1512,10 +1551,13 @@
       <c r="G36" t="b">
         <v>1</v>
       </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
@@ -1541,7 +1583,7 @@
       </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R37" s="12"/>
@@ -1566,10 +1608,13 @@
       <c r="G38" t="b">
         <v>1</v>
       </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R38" s="12"/>
       <c r="S38" s="13"/>
@@ -1586,7 +1631,7 @@
       </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R39" s="14"/>
@@ -1608,10 +1653,13 @@
       <c r="G40" t="b">
         <v>1</v>
       </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
@@ -1629,7 +1677,7 @@
       </c>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R41" s="12"/>
@@ -1645,7 +1693,7 @@
       </c>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R42" s="12"/>
@@ -1667,10 +1715,13 @@
       <c r="G43" t="b">
         <v>1</v>
       </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="13"/>
@@ -1683,10 +1734,13 @@
       <c r="F44" t="b">
         <v>1</v>
       </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R44" s="12"/>
       <c r="S44" s="13"/>
@@ -1704,7 +1758,7 @@
       </c>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R45" s="12"/>
@@ -1726,7 +1780,7 @@
       </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R46" s="12"/>
@@ -1747,7 +1801,7 @@
       </c>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R47" s="12"/>
@@ -1758,7 +1812,7 @@
       <c r="C48" s="10"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f t="shared" ref="Q45:Q50" si="0">C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
+        <f t="shared" ref="Q48:Q50" si="1">C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1769,7 +1823,7 @@
       <c r="C49" s="10"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="14"/>
@@ -1792,7 +1846,7 @@
       <c r="O50" s="19"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="21"/>

</xml_diff>

<commit_message>
Laborator 04.04 - Jocul Minesweeper, folosind Parcurgerea in Adancime
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAEF8E2-20B4-44A6-8321-DEB565B1EF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6BCC12-CCDE-4690-9DF6-08945D5E8E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -936,10 +936,13 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="13"/>
@@ -952,10 +955,13 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
@@ -974,10 +980,13 @@
       <c r="F9" t="b">
         <v>1</v>
       </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="13"/>
@@ -1084,10 +1093,13 @@
       <c r="G14" t="b">
         <v>1</v>
       </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="13"/>
@@ -1118,10 +1130,13 @@
       <c r="G16" t="b">
         <v>1</v>
       </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
@@ -1134,10 +1149,13 @@
       <c r="G17" t="b">
         <v>1</v>
       </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
@@ -1312,10 +1330,13 @@
       <c r="G25" t="b">
         <v>1</v>
       </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
@@ -1377,10 +1398,13 @@
       <c r="G28" t="b">
         <v>1</v>
       </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
@@ -1441,10 +1465,13 @@
       <c r="G31" t="b">
         <v>1</v>
       </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R31" s="12"/>
       <c r="S31" s="13"/>
@@ -1456,10 +1483,13 @@
       <c r="C32" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
@@ -1581,10 +1611,13 @@
       <c r="G37" t="b">
         <v>1</v>
       </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
@@ -1675,10 +1708,13 @@
       <c r="F41" t="b">
         <v>1</v>
       </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="11"/>
       <c r="Q41" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R41" s="12"/>
       <c r="S41" s="13"/>
@@ -1691,10 +1727,13 @@
       <c r="G42" t="b">
         <v>1</v>
       </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R42" s="12"/>
       <c r="S42" s="13"/>
@@ -1756,10 +1795,13 @@
       <c r="G45" t="b">
         <v>1</v>
       </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R45" s="12"/>
       <c r="S45" s="13"/>
@@ -1778,10 +1820,13 @@
       <c r="G46" t="b">
         <v>1</v>
       </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13"/>
@@ -1799,10 +1844,13 @@
       <c r="G47" t="b">
         <v>1</v>
       </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R47" s="12"/>
       <c r="S47" s="13"/>

</xml_diff>

<commit_message>
Laborator 09.04.2024 - am inceput realizarea unui joc Tower Defence
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6BCC12-CCDE-4690-9DF6-08945D5E8E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EE9937-12B5-475A-AA46-14DEECF63B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -834,7 +834,9 @@
         <v>1</v>
       </c>
       <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -844,7 +846,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
         <f t="shared" ref="Q3:Q47" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="9"/>
@@ -891,10 +893,13 @@
       <c r="H5" t="b">
         <v>1</v>
       </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
@@ -915,10 +920,13 @@
       <c r="G6" t="b">
         <v>1</v>
       </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R6" s="14"/>
       <c r="S6" s="15"/>
@@ -1029,10 +1037,13 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R11" s="12"/>
       <c r="S11" s="13"/>
@@ -1179,10 +1190,13 @@
       <c r="H18" t="b">
         <v>1</v>
       </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
@@ -1206,10 +1220,13 @@
       <c r="H19" t="b">
         <v>1</v>
       </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
@@ -1314,10 +1331,13 @@
       <c r="H24" t="b">
         <v>1</v>
       </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
@@ -1428,10 +1448,13 @@
       <c r="H29" t="b">
         <v>1</v>
       </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R29" s="12"/>
       <c r="S29" s="13"/>
@@ -1537,10 +1560,13 @@
       <c r="G34" t="b">
         <v>1</v>
       </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
@@ -1559,10 +1585,13 @@
       <c r="H35" t="b">
         <v>1</v>
       </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
@@ -1584,10 +1613,13 @@
       <c r="H36" t="b">
         <v>1</v>
       </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
@@ -1644,10 +1676,13 @@
       <c r="H38" t="b">
         <v>1</v>
       </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R38" s="12"/>
       <c r="S38" s="13"/>
@@ -1689,10 +1724,13 @@
       <c r="H40" t="b">
         <v>1</v>
       </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
@@ -1823,10 +1861,13 @@
       <c r="H46" t="b">
         <v>1</v>
       </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13"/>

</xml_diff>

<commit_message>
Laborator 23.04.2024 - am adaugat tower-urile si le putem misca dupa mouse
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57D856F-6CEE-4D76-925A-811B6C0C583C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D72DD-576E-4BAC-B363-0887B4C23C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -548,7 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
@@ -876,16 +875,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="22" customWidth="1"/>
-    <col min="18" max="18" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="22" customWidth="1"/>
+    <col min="18" max="18" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
@@ -973,7 +972,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q34" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>5</v>
       </c>
       <c r="R3" s="8"/>
@@ -984,27 +983,19 @@
         <v>55</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="26"/>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
       <c r="J4" s="24"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="7">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R4" s="12"/>
@@ -1015,43 +1006,41 @@
         <v>46</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="26" t="b">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="24"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
@@ -1067,13 +1056,13 @@
       <c r="M6" s="24"/>
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="35">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>1</v>
-      </c>
-      <c r="R6" s="27"/>
-      <c r="S6" s="28"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R6" s="26"/>
+      <c r="S6" s="27"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
@@ -1082,32 +1071,25 @@
       <c r="C7" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26" t="b">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R7" s="14"/>
@@ -1120,30 +1102,22 @@
       <c r="C8" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="26"/>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
       <c r="J8" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R8" s="12"/>
@@ -1154,27 +1128,18 @@
         <v>53</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="26"/>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
       <c r="J9" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="7">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R9" s="12"/>
@@ -1185,31 +1150,24 @@
         <v>41</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="26"/>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
       <c r="J10" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="7">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R10" s="12"/>
@@ -1220,23 +1178,13 @@
         <v>57</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
       <c r="J11" s="24"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="7">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R11" s="12"/>
@@ -1249,36 +1197,34 @@
       <c r="C12" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="26" t="b">
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="7">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="13"/>
@@ -1290,30 +1236,22 @@
       <c r="C13" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26" t="b">
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R13" s="12"/>
@@ -1326,27 +1264,19 @@
       <c r="C14" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="26"/>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
       <c r="J14" s="24"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R14" s="12"/>
@@ -1357,29 +1287,22 @@
         <v>43</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="26" t="b">
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" s="24"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R15" s="12"/>
@@ -1392,23 +1315,13 @@
       <c r="C16" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
       <c r="J16" s="24"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R16" s="12"/>
@@ -1419,30 +1332,22 @@
         <v>62</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="26" t="b">
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R17" s="12"/>
@@ -1453,25 +1358,16 @@
         <v>58</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="26"/>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
       <c r="J18" s="24"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R18" s="12"/>
@@ -1484,35 +1380,32 @@
       <c r="C19" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D19" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="26" t="b">
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
@@ -1524,35 +1417,32 @@
       <c r="C20" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="26" t="b">
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
@@ -1564,29 +1454,22 @@
       <c r="C21" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26" t="b">
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="24"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R21" s="12"/>
@@ -1597,36 +1480,26 @@
         <v>56</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
       <c r="J22" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1642,40 +1515,32 @@
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="35">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
-      </c>
-      <c r="R23" s="27"/>
-      <c r="S23" s="28"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R23" s="26"/>
+      <c r="S23" s="27"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="26"/>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
       <c r="J24" s="24"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R24" s="12"/>
@@ -1686,28 +1551,19 @@
         <v>52</v>
       </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="26"/>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
       <c r="J25" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R25" s="12"/>
@@ -1720,34 +1576,28 @@
       <c r="C26" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="26" t="b">
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
         <v>1</v>
       </c>
       <c r="J26" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="R26" s="12"/>
@@ -1758,27 +1608,19 @@
         <v>60</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="26" t="b">
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="24"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R27" s="12"/>
@@ -1789,32 +1631,25 @@
         <v>48</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="26"/>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
       <c r="J28" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R28" s="12"/>
@@ -1827,29 +1662,21 @@
       <c r="C29" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="26"/>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="J29" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="7">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R29" s="12"/>
@@ -1860,38 +1687,29 @@
         <v>59</v>
       </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="26"/>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
       <c r="J30" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="27"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -1907,13 +1725,13 @@
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="35">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>1</v>
-      </c>
-      <c r="R31" s="27"/>
-      <c r="S31" s="28"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R31" s="26"/>
+      <c r="S31" s="27"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
@@ -1922,35 +1740,32 @@
       <c r="C32" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="26" t="b">
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
         <v>1</v>
       </c>
       <c r="J32" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="7">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="R32" s="12"/>
       <c r="S32" s="13"/>
@@ -1960,23 +1775,13 @@
         <v>50</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
       <c r="J33" s="24"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R33" s="12"/>
@@ -1989,27 +1794,19 @@
       <c r="C34" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="26"/>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
       <c r="J34" s="24"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R34" s="12"/>
@@ -2022,27 +1819,18 @@
       <c r="C35" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="26" t="b">
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="b">
         <v>1</v>
       </c>
       <c r="J35" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>4</v>
       </c>
       <c r="R35" s="12"/>
@@ -2055,34 +1843,28 @@
       <c r="C36" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D36" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26" t="b">
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
         <v>1</v>
       </c>
       <c r="J36" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R36" s="12"/>
@@ -2095,39 +1877,32 @@
       <c r="C37" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D37" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26" t="b">
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
         <v>1</v>
       </c>
       <c r="J37" s="24"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
     </row>
     <row r="38" spans="2:19">
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="27"/>
+      <c r="C38" s="26"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -2143,42 +1918,35 @@
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
       <c r="O38" s="24"/>
-      <c r="P38" s="28"/>
-      <c r="Q38" s="35">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>1</v>
-      </c>
-      <c r="R38" s="30"/>
-      <c r="S38" s="31"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R38" s="29"/>
+      <c r="S38" s="30"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="26" t="b">
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" s="24"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R39" s="12"/>
@@ -2189,43 +1957,37 @@
         <v>47</v>
       </c>
       <c r="C40" s="10"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="26" t="b">
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
-      <c r="M40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="27"/>
+      <c r="C41" s="26"/>
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -2241,13 +2003,13 @@
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
       <c r="O41" s="24"/>
-      <c r="P41" s="28"/>
-      <c r="Q41" s="35">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>1</v>
-      </c>
-      <c r="R41" s="32"/>
-      <c r="S41" s="31"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="31"/>
+      <c r="S41" s="30"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="3" t="s">
@@ -2256,36 +2018,34 @@
       <c r="C42" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D42" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" s="26" t="b">
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
         <v>1</v>
       </c>
       <c r="J42" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="26"/>
-      <c r="N42" s="26"/>
-      <c r="O42" s="26"/>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="11"/>
       <c r="Q42" s="7">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="R42" s="12"/>
       <c r="S42" s="13"/>
@@ -2297,34 +2057,32 @@
       <c r="C43" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D43" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G43" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" s="26" t="b">
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" s="24"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="13"/>
@@ -2336,26 +2094,16 @@
       <c r="C44" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
       <c r="J44" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
-      <c r="M44" s="26"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="R44" s="14"/>
@@ -2368,35 +2116,32 @@
       <c r="C45" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D45" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G45" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" s="26" t="b">
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
         <v>1</v>
       </c>
       <c r="J45" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
-        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="R45" s="12"/>
       <c r="S45" s="13"/>
@@ -2406,31 +2151,24 @@
         <v>49</v>
       </c>
       <c r="C46" s="10"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I46" s="26" t="b">
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="26"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
-        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R46" s="12"/>
@@ -2441,29 +2179,21 @@
         <v>61</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" s="26" t="b">
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
         <v>1</v>
       </c>
       <c r="J47" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="26"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
-        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R47" s="12"/>
@@ -2476,173 +2206,135 @@
       <c r="C48" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G48" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48" s="26" t="b">
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
         <v>1</v>
       </c>
       <c r="J48" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="26"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
-        <f>C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R48" s="12"/>
       <c r="S48" s="13"/>
     </row>
     <row r="49" spans="2:19">
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="33" t="s">
         <v>51</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" s="26" t="b">
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="26"/>
       <c r="P49" s="11"/>
-      <c r="Q49" s="36">
-        <f>C49+D49+E49+F49+G49+H49+I49+J49+K49+L49+M49+N49+O49+P49</f>
+      <c r="Q49" s="35">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R49" s="12"/>
       <c r="S49" s="13"/>
     </row>
     <row r="50" spans="2:19">
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="33" t="s">
         <v>54</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G50" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H50" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I50" s="26"/>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
       <c r="J50" s="24"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="26"/>
       <c r="P50" s="11"/>
-      <c r="Q50" s="36">
-        <f>C50+D50+E50+F50+G50+H50+I50+J50+K50+L50+M50+N50+O50+P50</f>
+      <c r="Q50" s="35">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="R50" s="12"/>
       <c r="S50" s="13"/>
     </row>
     <row r="51" spans="2:19">
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="33" t="s">
         <v>63</v>
       </c>
       <c r="C51" s="10"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26" t="b">
+      <c r="I51" t="b">
         <v>1</v>
       </c>
       <c r="J51" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="26"/>
       <c r="P51" s="11"/>
-      <c r="Q51" s="36">
-        <f>C51+D51+E51+F51+G51+H51+I51+J51+K51+L51+M51+N51+O51+P51</f>
+      <c r="Q51" s="35">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R51" s="12"/>
       <c r="S51" s="13"/>
     </row>
     <row r="52" spans="2:19">
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="33" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G52" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H52" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I52" s="26" t="b">
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
         <v>1</v>
       </c>
       <c r="J52" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="26"/>
-      <c r="N52" s="26"/>
-      <c r="O52" s="26"/>
       <c r="P52" s="11"/>
-      <c r="Q52" s="36">
-        <f>C52+D52+E52+F52+G52+H52+I52+J52+K52+L52+M52+N52+O52+P52</f>
+      <c r="Q52" s="35">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R52" s="12"/>
       <c r="S52" s="13"/>
     </row>
     <row r="53" spans="2:19">
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="33" t="s">
         <v>36</v>
       </c>
       <c r="C53" s="17" t="b">
@@ -2660,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="18"/>
-      <c r="J53" s="29" t="b">
+      <c r="J53" s="28" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -2670,8 +2362,8 @@
       <c r="N53" s="18"/>
       <c r="O53" s="18"/>
       <c r="P53" s="19"/>
-      <c r="Q53" s="36">
-        <f>C53+D53+E53+F53+G53+H53+I53+J53+K53+L53+M53+N53+O53+P53</f>
+      <c r="Q53" s="35">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R53" s="20"/>

</xml_diff>

<commit_message>
am adaugat clasa Engine
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D72DD-576E-4BAC-B363-0887B4C23C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5696FC61-E62A-4766-9999-FA103A198110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Proiect</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>David Pit</t>
+  </si>
+  <si>
+    <t>Casian Balaj</t>
   </si>
 </sst>
 </file>
@@ -311,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -488,12 +491,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,6 +582,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -873,18 +888,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S53"/>
+  <dimension ref="B2:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="22" customWidth="1"/>
-    <col min="18" max="18" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="22" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
@@ -1115,10 +1130,13 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R8" s="12"/>
       <c r="S8" s="13"/>
@@ -1300,10 +1318,13 @@
         <v>1</v>
       </c>
       <c r="J15" s="24"/>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
@@ -1538,10 +1559,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="24"/>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R24" s="12"/>
       <c r="S24" s="13"/>
@@ -1804,10 +1828,13 @@
         <v>1</v>
       </c>
       <c r="J34" s="24"/>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
@@ -1830,7 +1857,7 @@
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" ref="Q35:Q54" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>4</v>
       </c>
       <c r="R35" s="12"/>
@@ -1975,10 +2002,13 @@
       <c r="J40" s="24" t="b">
         <v>1</v>
       </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
@@ -2166,10 +2196,13 @@
       <c r="J46" s="24" t="b">
         <v>1</v>
       </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13"/>
@@ -2273,10 +2306,13 @@
         <v>1</v>
       </c>
       <c r="J50" s="24"/>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
       <c r="P50" s="11"/>
       <c r="Q50" s="35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R50" s="12"/>
       <c r="S50" s="13"/>
@@ -2356,7 +2392,9 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K53" s="18"/>
+      <c r="K53" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="L53" s="18"/>
       <c r="M53" s="18"/>
       <c r="N53" s="18"/>
@@ -2364,10 +2402,22 @@
       <c r="P53" s="19"/>
       <c r="Q53" s="35">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R53" s="20"/>
       <c r="S53" s="21"/>
+    </row>
+    <row r="54" spans="2:19">
+      <c r="B54" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K54" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S53">
@@ -2378,7 +2428,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q49:Q53">
+  <conditionalFormatting sqref="Q49:Q54">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Laborator 14.05.2024 - am adaugat imagini, acum putem plasa towers, selecta si deselecta tower-urile plasate precedent
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5696FC61-E62A-4766-9999-FA103A198110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E9AB51-648A-408B-B33D-FC0462B44141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,9 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -505,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,6 +587,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -890,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,13 +987,15 @@
       <c r="J3" s="25"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="M3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
         <f t="shared" ref="Q3:Q34" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="9"/>
@@ -1043,10 +1050,13 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
@@ -1102,10 +1112,13 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
@@ -1267,44 +1280,44 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="L13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" s="12"/>
       <c r="S13" s="13"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C14" s="10"/>
       <c r="J14" s="24"/>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R14" s="12"/>
-      <c r="S14" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="R14" s="10"/>
+      <c r="S14" s="11"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
@@ -1314,69 +1327,69 @@
       <c r="H15" t="b">
         <v>1</v>
       </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
       <c r="J15" s="24"/>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R15" s="12"/>
       <c r="S15" s="13"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
+        <v>43</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="b">
         <v>1</v>
       </c>
       <c r="J16" s="24"/>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="24" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C17" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="24"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C18" s="10"/>
       <c r="G18" t="b">
@@ -1385,55 +1398,44 @@
       <c r="H18" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="24"/>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="24" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R18" s="12"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
+        <v>58</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" s="24" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K19" t="b">
-        <v>1</v>
-      </c>
+      <c r="J19" s="24"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R19" s="12"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C20" s="10" t="b">
         <v>1</v>
@@ -1441,10 +1443,10 @@
       <c r="D20" t="b">
         <v>1</v>
       </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
       <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="H20" t="b">
@@ -1460,17 +1462,20 @@
       <c r="K20" t="b">
         <v>1</v>
       </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R20" s="12"/>
       <c r="S20" s="13"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C21" s="10" t="b">
         <v>1</v>
@@ -1484,135 +1489,144 @@
       <c r="G21" t="b">
         <v>1</v>
       </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="24" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R21" s="12"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="C22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="24" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="24"/>
       <c r="P22" s="11"/>
       <c r="Q22" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R22" s="12"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
+      <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
       <c r="J23" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R23" s="26"/>
-      <c r="S23" s="27"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R23" s="12"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="24"/>
-      <c r="K24" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R24" s="12"/>
-      <c r="S24" s="13"/>
+      <c r="B24" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R24" s="26"/>
+      <c r="S24" s="27"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C25" s="10"/>
-      <c r="F25" t="b">
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
         <v>1</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="24" t="b">
-        <f>TRUE()</f>
+      <c r="J25" s="24"/>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R25" s="12"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C26" s="10"/>
       <c r="F26" t="b">
         <v>1</v>
       </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
       <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="b">
         <v>1</v>
       </c>
       <c r="J26" s="24" t="b">
@@ -1622,16 +1636,24 @@
       <c r="P26" s="11"/>
       <c r="Q26" s="7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R26" s="12"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C27" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
@@ -1641,61 +1663,66 @@
       <c r="I27" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="24"/>
+      <c r="J27" s="24" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R27" s="12"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
       <c r="G28" t="b">
         <v>1</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
       </c>
-      <c r="J28" s="24" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="24"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="13"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="10" t="b">
-        <v>1</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C29" s="10"/>
       <c r="E29" t="b">
         <v>1</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
       </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
       <c r="H29" t="b">
         <v>1</v>
       </c>
       <c r="J29" s="24" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P29" s="11"/>
@@ -1708,198 +1735,197 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="G30" t="b">
+        <v>29</v>
+      </c>
+      <c r="C30" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
         <v>1</v>
       </c>
       <c r="H30" t="b">
         <v>1</v>
       </c>
       <c r="J30" s="24" t="b">
-        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R30" s="12"/>
       <c r="S30" s="13"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="B31" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
+      <c r="B31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
       <c r="J31" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R31" s="26"/>
-      <c r="S31" s="27"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R31" s="12"/>
+      <c r="S31" s="13"/>
     </row>
     <row r="32" spans="2:19">
-      <c r="B32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
+      <c r="B32" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K32" t="b">
-        <v>1</v>
-      </c>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="7">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R32" s="12"/>
-      <c r="S32" s="13"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R32" s="26"/>
+      <c r="S32" s="27"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="C33" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
       <c r="F33" t="b">
         <v>1</v>
       </c>
-      <c r="J33" s="24"/>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="24" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="R33" s="12"/>
       <c r="S33" s="13"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G34" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" t="b">
+        <v>50</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="F34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="24"/>
-      <c r="K34" t="b">
-        <v>1</v>
-      </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R34" s="12"/>
       <c r="S34" s="13"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C35" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
       <c r="H35" t="b">
         <v>1</v>
       </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" s="24" t="b">
+      <c r="J35" s="24"/>
+      <c r="K35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="7">
-        <f t="shared" ref="Q35:Q54" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>4</v>
+        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>5</v>
       </c>
       <c r="R35" s="12"/>
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C36" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
+      <c r="H36" t="b">
         <v>1</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
       </c>
       <c r="J36" s="24" t="b">
-        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R36" s="12"/>
       <c r="S36" s="13"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C37" s="10" t="b">
         <v>1</v>
@@ -1907,6 +1933,9 @@
       <c r="D37" t="b">
         <v>1</v>
       </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
       <c r="F37" t="b">
         <v>1</v>
       </c>
@@ -1916,173 +1945,170 @@
       <c r="I37" t="b">
         <v>1</v>
       </c>
-      <c r="J37" s="24"/>
+      <c r="J37" s="24" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R37" s="12"/>
       <c r="S37" s="13"/>
     </row>
     <row r="38" spans="2:19">
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="24"/>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="R38" s="12"/>
+      <c r="S38" s="13"/>
+    </row>
+    <row r="39" spans="2:19">
+      <c r="B39" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24" t="b">
+      <c r="C39" s="26"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="34">
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="34">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R38" s="29"/>
-      <c r="S38" s="30"/>
-    </row>
-    <row r="39" spans="2:19">
-      <c r="B39" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" s="24"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R39" s="12"/>
-      <c r="S39" s="13"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="30"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" s="10"/>
-      <c r="E40" t="b">
+      <c r="D40" t="b">
         <v>1</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
       </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
       <c r="H40" t="b">
         <v>1</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
-      <c r="J40" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K40" t="b">
-        <v>1</v>
-      </c>
+      <c r="J40" s="24"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13"/>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R41" s="12"/>
+      <c r="S41" s="13"/>
+    </row>
+    <row r="42" spans="2:19">
+      <c r="B42" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24" t="b">
+      <c r="C42" s="26"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="34">
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="34">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R41" s="31"/>
-      <c r="S41" s="30"/>
-    </row>
-    <row r="42" spans="2:19">
-      <c r="B42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" t="b">
-        <v>1</v>
-      </c>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="7">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="R42" s="12"/>
-      <c r="S42" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="R42" s="31"/>
+      <c r="S42" s="30"/>
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C43" s="10" t="b">
         <v>1</v>
@@ -2105,88 +2131,98 @@
       <c r="I43" t="b">
         <v>1</v>
       </c>
-      <c r="J43" s="24"/>
+      <c r="J43" s="24" t="b">
+        <v>1</v>
+      </c>
       <c r="K43" t="b">
         <v>1</v>
       </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R43" s="12"/>
       <c r="S43" s="13"/>
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C44" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
       <c r="G44" t="b">
         <v>1</v>
       </c>
-      <c r="J44" s="24" t="b">
-        <f>TRUE()</f>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="24"/>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+      <c r="M44" t="b">
         <v>1</v>
       </c>
       <c r="P44" s="11"/>
       <c r="Q44" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="R44" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="R44" s="12"/>
       <c r="S44" s="13"/>
     </row>
     <row r="45" spans="2:19">
       <c r="B45" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C45" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
       <c r="G45" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" t="b">
         <v>1</v>
       </c>
       <c r="J45" s="24" t="b">
         <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K45" t="b">
         <v>1</v>
       </c>
       <c r="P45" s="11"/>
       <c r="Q45" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="R45" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="R45" s="14"/>
       <c r="S45" s="13"/>
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="E46" t="b">
+        <v>35</v>
+      </c>
+      <c r="C46" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" t="b">
         <v>1</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
       </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
       <c r="H46" t="b">
         <v>1</v>
       </c>
@@ -2194,25 +2230,35 @@
         <v>1</v>
       </c>
       <c r="J46" s="24" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+      <c r="M46" t="b">
         <v>1</v>
       </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R46" s="12"/>
       <c r="S46" s="13"/>
     </row>
     <row r="47" spans="2:19">
       <c r="B47" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="G47" t="b">
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
         <v>1</v>
       </c>
       <c r="H47" t="b">
@@ -2222,29 +2268,27 @@
         <v>1</v>
       </c>
       <c r="J47" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" t="b">
         <v>1</v>
       </c>
       <c r="P47" s="11"/>
       <c r="Q47" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R47" s="12"/>
       <c r="S47" s="13"/>
     </row>
     <row r="48" spans="2:19">
       <c r="B48" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" t="b">
-        <v>1</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C48" s="10"/>
       <c r="G48" t="b">
         <v>1</v>
       </c>
@@ -2255,25 +2299,32 @@
         <v>1</v>
       </c>
       <c r="J48" s="24" t="b">
-        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P48" s="11"/>
       <c r="Q48" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R48" s="12"/>
       <c r="S48" s="13"/>
     </row>
     <row r="49" spans="2:19">
       <c r="B49" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="C49" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
       <c r="F49" t="b">
         <v>1</v>
       </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
       <c r="H49" t="b">
         <v>1</v>
       </c>
@@ -2281,32 +2332,32 @@
         <v>1</v>
       </c>
       <c r="J49" s="24" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P49" s="11"/>
       <c r="Q49" s="35">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R49" s="12"/>
       <c r="S49" s="13"/>
     </row>
     <row r="50" spans="2:19">
       <c r="B50" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C50" s="10"/>
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="G50" t="b">
-        <v>1</v>
-      </c>
       <c r="H50" t="b">
         <v>1</v>
       </c>
-      <c r="J50" s="24"/>
-      <c r="K50" t="b">
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" s="24" t="b">
         <v>1</v>
       </c>
       <c r="P50" s="11"/>
@@ -2319,41 +2370,35 @@
     </row>
     <row r="51" spans="2:19">
       <c r="B51" s="33" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C51" s="10"/>
-      <c r="I51" t="b">
-        <v>1</v>
-      </c>
-      <c r="J51" s="24" t="b">
-        <f>TRUE()</f>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" s="24"/>
+      <c r="K51" t="b">
         <v>1</v>
       </c>
       <c r="P51" s="11"/>
       <c r="Q51" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R51" s="12"/>
       <c r="S51" s="13"/>
     </row>
     <row r="52" spans="2:19">
       <c r="B52" s="33" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" t="b">
-        <v>1</v>
-      </c>
-      <c r="G52" t="b">
-        <v>1</v>
-      </c>
-      <c r="H52" t="b">
-        <v>1</v>
-      </c>
       <c r="I52" t="b">
         <v>1</v>
       </c>
@@ -2364,64 +2409,87 @@
       <c r="P52" s="11"/>
       <c r="Q52" s="35">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R52" s="12"/>
       <c r="S52" s="13"/>
     </row>
     <row r="53" spans="2:19">
-      <c r="B53" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G53" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I53" s="18"/>
-      <c r="J53" s="28" t="b">
+      <c r="B53" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="J53" s="24" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K53" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="19"/>
+      <c r="L53" t="b">
+        <v>1</v>
+      </c>
+      <c r="P53" s="11"/>
       <c r="Q53" s="35">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="R53" s="20"/>
-      <c r="S53" s="21"/>
+        <v>7</v>
+      </c>
+      <c r="R53" s="12"/>
+      <c r="S53" s="13"/>
     </row>
     <row r="54" spans="2:19">
-      <c r="B54" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="K54" t="b">
-        <v>1</v>
-      </c>
+      <c r="B54" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="18"/>
+      <c r="J54" s="28" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="19"/>
       <c r="Q54" s="35">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="R54" s="20"/>
+      <c r="S54" s="21"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S53">
-    <sortCondition ref="B53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S54">
+    <sortCondition ref="B54"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q48">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
Notele finale (dupa "restante")
</commit_message>
<xml_diff>
--- a/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
+++ b/AlgoritmiFundamentali/Prezenta_AnI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2024\AlgoritmiFundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAD51DA-6CD9-473D-A022-93D75F06E418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0148E8FD-1D7B-4C81-92E0-E4B401D19B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>Proiect</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>Picture puzzle</t>
+  </si>
+  <si>
+    <t>Tank Shooter</t>
+  </si>
+  <si>
+    <t>Biliard</t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,16 +667,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -977,10 +980,10 @@
   <dimension ref="B2:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S37" sqref="S37"/>
+      <selection pane="bottomRight" activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,8 +991,8 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="21" customWidth="1"/>
-    <col min="18" max="18" width="27.42578125" style="38" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="38"/>
+    <col min="18" max="18" width="27.42578125" style="37" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="37"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
@@ -1184,14 +1187,18 @@
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="26"/>
+      <c r="P6" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="Q6" s="33">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R6" s="28"/>
-      <c r="S6" s="39">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="R6" s="28">
+        <v>2048</v>
+      </c>
+      <c r="S6" s="38">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:19">
@@ -1856,14 +1863,18 @@
       <c r="M26" s="23"/>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
-      <c r="P26" s="26"/>
+      <c r="P26" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="Q26" s="33">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R26" s="28"/>
-      <c r="S26" s="39">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="S26" s="38">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:19">
@@ -1976,7 +1987,7 @@
         <v>73</v>
       </c>
       <c r="S29" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:19">
@@ -2045,284 +2056,272 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" s="23" t="b">
-        <v>1</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="J32" s="23"/>
       <c r="P32" s="11" t="b">
         <v>1</v>
       </c>
       <c r="Q32" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R32" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="S32" s="13">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="R32" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="S32" s="15">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="G33" t="b">
+        <v>29</v>
+      </c>
+      <c r="C33" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
         <v>1</v>
       </c>
       <c r="H33" t="b">
         <v>1</v>
       </c>
       <c r="J33" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P33" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="P33" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q33" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R33" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="R33" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="S33" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="2:19">
-      <c r="B34" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
+      <c r="B34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
       <c r="J34" s="23" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="O34" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P34" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="33">
+      <c r="P34" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R34" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="S34" s="39">
-        <v>8</v>
+      <c r="R34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="S34" s="13">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:19">
-      <c r="B35" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
+      <c r="B35" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
       <c r="J35" s="23" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K35" t="b">
-        <v>1</v>
-      </c>
-      <c r="L35" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" t="b">
-        <v>1</v>
-      </c>
-      <c r="N35" t="b">
-        <v>1</v>
-      </c>
-      <c r="O35" t="b">
-        <v>1</v>
-      </c>
-      <c r="P35" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="7">
-        <f t="shared" ref="Q35:Q57" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>13</v>
-      </c>
-      <c r="R35" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="S35" s="13">
-        <v>10</v>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="33">
+        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>4</v>
+      </c>
+      <c r="R35" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="S35" s="38">
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="C36" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
       <c r="F36" t="b">
         <v>1</v>
       </c>
-      <c r="J36" s="23"/>
-      <c r="P36" s="11"/>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q36" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R36" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="R36" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="S36" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="b">
+        <v>50</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="F37" t="b">
         <v>1</v>
       </c>
       <c r="J37" s="23"/>
-      <c r="K37" t="b">
-        <v>1</v>
-      </c>
-      <c r="N37" t="b">
-        <v>1</v>
-      </c>
-      <c r="P37" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="P37" s="11"/>
       <c r="Q37" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="R37" s="12" t="s">
-        <v>78</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R37" s="12"/>
       <c r="S37" s="13">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C38" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
       <c r="H38" t="b">
         <v>1</v>
       </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L38" t="b">
-        <v>1</v>
-      </c>
-      <c r="O38" t="b">
-        <v>1</v>
-      </c>
-      <c r="P38" s="11"/>
+      <c r="J38" s="23"/>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q38" s="7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R38" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="S38" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C39" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" t="b">
+      <c r="H39" t="b">
         <v>1</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" s="23" t="b">
-        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="R39" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="S39" s="13">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C40" s="10" t="b">
         <v>1</v>
@@ -2330,6 +2329,9 @@
       <c r="D40" t="b">
         <v>1</v>
       </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
       <c r="F40" t="b">
         <v>1</v>
       </c>
@@ -2339,14 +2341,14 @@
       <c r="I40" t="b">
         <v>1</v>
       </c>
-      <c r="J40" s="23"/>
-      <c r="M40" t="b">
+      <c r="J40" s="23" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R40" s="12"/>
       <c r="S40" s="13">
@@ -2354,192 +2356,177 @@
       </c>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" s="23"/>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="R41" s="12"/>
+      <c r="S41" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19">
+      <c r="B42" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23" t="b">
+      <c r="C42" s="25"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="33">
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="33">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R41" s="28"/>
-      <c r="S41" s="29">
+      <c r="R42" s="28"/>
+      <c r="S42" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:19">
-      <c r="B42" s="3" t="s">
+    <row r="43" spans="2:19">
+      <c r="B43" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" s="23"/>
-      <c r="P42" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="7">
+      <c r="C43" s="10"/>
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" s="23"/>
+      <c r="P43" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="R42" s="12" t="s">
+      <c r="R43" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="S42" s="13">
+      <c r="S43" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="2:19">
-      <c r="B43" s="3" t="s">
+    <row r="44" spans="2:19">
+      <c r="B44" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G43" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" t="b">
-        <v>1</v>
-      </c>
-      <c r="J43" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K43" t="b">
-        <v>1</v>
-      </c>
-      <c r="P43" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="7">
+      <c r="C44" s="10"/>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="7">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="R43" s="12" t="s">
+      <c r="R44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="S43" s="13">
+      <c r="S44" s="13">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="2:19">
-      <c r="B44" s="37" t="s">
+    <row r="45" spans="2:19">
+      <c r="B45" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23" t="b">
+      <c r="C45" s="25"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N44" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="O44" s="23"/>
-      <c r="P44" s="26"/>
-      <c r="Q44" s="33">
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N45" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45" s="23"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="33">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="R44" s="30"/>
-      <c r="S44" s="29">
+      <c r="R45" s="30"/>
+      <c r="S45" s="29">
         <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:19">
-      <c r="B45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
-      <c r="G45" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" t="b">
-        <v>1</v>
-      </c>
-      <c r="J45" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K45" t="b">
-        <v>1</v>
-      </c>
-      <c r="M45" t="b">
-        <v>1</v>
-      </c>
-      <c r="P45" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="7">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="R45" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="S45" s="13">
-        <v>10</v>
       </c>
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C46" s="10" t="b">
         <v>1</v>
@@ -2562,107 +2549,102 @@
       <c r="I46" t="b">
         <v>1</v>
       </c>
-      <c r="J46" s="23"/>
+      <c r="J46" s="23" t="b">
+        <v>1</v>
+      </c>
       <c r="K46" t="b">
         <v>1</v>
       </c>
       <c r="M46" t="b">
         <v>1</v>
       </c>
-      <c r="N46" t="b">
-        <v>1</v>
-      </c>
-      <c r="O46" t="b">
-        <v>1</v>
-      </c>
-      <c r="P46" s="11"/>
+      <c r="P46" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q46" s="7">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="R46" s="12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="S46" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="2:19">
       <c r="B47" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C47" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
       <c r="G47" t="b">
         <v>1</v>
       </c>
-      <c r="J47" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P47" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" s="23"/>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+      <c r="M47" t="b">
+        <v>1</v>
+      </c>
+      <c r="N47" t="b">
+        <v>1</v>
+      </c>
+      <c r="O47" t="b">
+        <v>1</v>
+      </c>
+      <c r="P47" s="11"/>
       <c r="Q47" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R47" s="14" t="s">
-        <v>88</v>
+        <v>11</v>
+      </c>
+      <c r="R47" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="S47" s="13">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="2:19">
       <c r="B48" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C48" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" t="b">
-        <v>1</v>
-      </c>
       <c r="G48" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48" t="b">
         <v>1</v>
       </c>
       <c r="J48" s="23" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K48" t="b">
-        <v>1</v>
-      </c>
-      <c r="L48" t="b">
-        <v>1</v>
-      </c>
-      <c r="M48" t="b">
-        <v>1</v>
-      </c>
-      <c r="N48" t="b">
-        <v>1</v>
-      </c>
-      <c r="O48" t="b">
-        <v>1</v>
-      </c>
-      <c r="P48" s="11"/>
+      <c r="P48" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q48" s="7">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="R48" s="12" t="s">
-        <v>78</v>
+        <v>4</v>
+      </c>
+      <c r="R48" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="S48" s="13">
         <v>10</v>
@@ -2670,15 +2652,20 @@
     </row>
     <row r="49" spans="2:19">
       <c r="B49" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="E49" t="b">
+        <v>35</v>
+      </c>
+      <c r="C49" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="b">
         <v>1</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
       </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
       <c r="H49" t="b">
         <v>1</v>
       </c>
@@ -2686,6 +2673,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="23" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="K49" t="b">
@@ -2703,26 +2691,27 @@
       <c r="O49" t="b">
         <v>1</v>
       </c>
-      <c r="P49" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="P49" s="11"/>
       <c r="Q49" s="34">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R49" s="12" t="s">
         <v>78</v>
       </c>
       <c r="S49" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="2:19">
       <c r="B50" s="32" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="G50" t="b">
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
         <v>1</v>
       </c>
       <c r="H50" t="b">
@@ -2734,29 +2723,40 @@
       <c r="J50" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="P50" s="11"/>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
+      <c r="L50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="N50" t="b">
+        <v>1</v>
+      </c>
+      <c r="O50" t="b">
+        <v>1</v>
+      </c>
+      <c r="P50" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q50" s="34">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R50" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="R50" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="S50" s="13">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:19">
       <c r="B51" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" t="b">
-        <v>1</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C51" s="10"/>
       <c r="G51" t="b">
         <v>1</v>
       </c>
@@ -2767,37 +2767,34 @@
         <v>1</v>
       </c>
       <c r="J51" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N51" t="b">
-        <v>1</v>
-      </c>
-      <c r="O51" t="b">
-        <v>1</v>
-      </c>
-      <c r="P51" s="11" t="b">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P51" s="11"/>
       <c r="Q51" s="34">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="R51" s="12" t="s">
-        <v>85</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="R51" s="12"/>
       <c r="S51" s="13">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="2:19">
       <c r="B52" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="C52" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
       <c r="F52" t="b">
         <v>1</v>
       </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
       <c r="H52" t="b">
         <v>1</v>
       </c>
@@ -2805,53 +2802,56 @@
         <v>1</v>
       </c>
       <c r="J52" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N52" t="b">
         <v>1</v>
       </c>
       <c r="O52" t="b">
         <v>1</v>
       </c>
-      <c r="P52" s="11"/>
+      <c r="P52" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q52" s="34">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R52" s="12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="S52" s="13">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="2:19">
       <c r="B53" s="35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C53" s="10"/>
       <c r="F53" t="b">
         <v>1</v>
       </c>
-      <c r="G53" t="b">
-        <v>1</v>
-      </c>
       <c r="H53" t="b">
         <v>1</v>
       </c>
-      <c r="J53" s="23"/>
-      <c r="K53" t="b">
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="J53" s="23" t="b">
         <v>1</v>
       </c>
       <c r="O53" t="b">
         <v>1</v>
       </c>
-      <c r="P53" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="P53" s="11"/>
       <c r="Q53" s="34">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R53" s="12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="S53" s="13">
         <v>10</v>
@@ -2859,20 +2859,20 @@
     </row>
     <row r="54" spans="2:19">
       <c r="B54" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="I54" t="b">
-        <v>1</v>
-      </c>
-      <c r="J54" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M54" t="b">
-        <v>1</v>
-      </c>
-      <c r="N54" t="b">
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54" s="23"/>
+      <c r="K54" t="b">
         <v>1</v>
       </c>
       <c r="O54" t="b">
@@ -2886,29 +2886,17 @@
         <v>6</v>
       </c>
       <c r="R54" s="12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S54" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="55" spans="2:19">
-      <c r="B55" s="36" t="s">
-        <v>44</v>
+      <c r="B55" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C55" s="10"/>
-      <c r="D55" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
-      </c>
-      <c r="G55" t="b">
-        <v>1</v>
-      </c>
-      <c r="H55" t="b">
-        <v>1</v>
-      </c>
       <c r="I55" t="b">
         <v>1</v>
       </c>
@@ -2916,10 +2904,13 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L55" t="b">
+      <c r="M55" t="b">
         <v>1</v>
       </c>
       <c r="N55" t="b">
+        <v>1</v>
+      </c>
+      <c r="O55" t="b">
         <v>1</v>
       </c>
       <c r="P55" s="11" t="b">
@@ -2927,78 +2918,104 @@
       </c>
       <c r="Q55" s="34">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R55" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S55" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="2:19">
-      <c r="B56" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G56" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I56" s="17"/>
-      <c r="J56" s="27" t="b">
+      <c r="B56" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" s="23" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K56" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="O56" s="17"/>
-      <c r="P56" s="18"/>
+      <c r="L56" t="b">
+        <v>1</v>
+      </c>
+      <c r="N56" t="b">
+        <v>1</v>
+      </c>
+      <c r="P56" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="Q56" s="34">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="R56" s="19"/>
-      <c r="S56" s="20">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="R56" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="S56" s="13">
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="2:19">
-      <c r="B57" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="P57" t="b">
-        <v>1</v>
-      </c>
+      <c r="B57" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="17"/>
+      <c r="J57" s="27" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K57" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O57" s="17"/>
+      <c r="P57" s="18"/>
       <c r="Q57" s="34">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R57" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="S57" s="38">
         <v>7</v>
       </c>
+      <c r="R57" s="19"/>
+      <c r="S57" s="20">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S56">
-    <sortCondition ref="B56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S57">
+    <sortCondition ref="B3:B57"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q48">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">

</xml_diff>